<commit_message>
chỉnh sửa nội dung theo yêu cầu
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Lap phieu thu/AF0061 Lap phieu thu.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Lap phieu thu/AF0061 Lap phieu thu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="824" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" tabRatio="824" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -1403,7 +1403,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="231">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2239,40 +2239,19 @@
     <t>@SQL0004</t>
   </si>
   <si>
-    <t>@DivisionID @ObjectID</t>
-  </si>
-  <si>
-    <t>@@DivisionID @@ObjectID</t>
-  </si>
-  <si>
     <t>Form</t>
   </si>
   <si>
     <t>Load</t>
   </si>
   <si>
-    <t>Nhận tham số từ màn hình AF0324 gọi màn hình AF0061 đồng thời load dữ liệu lên màn hình AF0061 từ đơn hàng khi thực thi @SQL0004</t>
-  </si>
-  <si>
     <t>ObjectID</t>
   </si>
   <si>
     <t>CustomizeIndex = 51</t>
   </si>
   <si>
-    <t>- Nhận tham số @DivisionID và @ObjectID gọi màn hình AF0061 và thực thi @SQL0004 để load form AF061</t>
-  </si>
-  <si>
-    <t>@DivisionID, @ObjectID</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ver 3.0 </t>
-  </si>
-  <si>
-    <t>- Chọn Btn Hóa đơn bán hàng truyền tham số @DivisionID và @ObjectID để gọi màn hình AF0274</t>
-  </si>
-  <si>
-    <t>- Customize cho Hoàng Trần (CustomizeIndex = 51): kế thừa hóa đơn bán hàng và load đơn hàng theo barcode từ tham số truyền vào</t>
   </si>
   <si>
     <t>OT2002, AT9000, AT2001</t>
@@ -2304,7 +2283,26 @@
 LEFT JOIN AT9000 AT00 ON AT00.DivisionID = OT02.DivisionID AND AT00.TransactionID = OT02.TransactionID
 INNER JOIN OT2001 OT01 ON OT01.DivisionID = OT02.DivisionID AND OT01.SOrderID = OT02.SOrderID
 LEFT JOIN At2007 ON (AT2007.InheritVoucherID = OT02.SOrderID  AND OT02.TransactionID = AT2007.InheritTransactionID) 
-      OR (AT2007.OTransactionID = OT02.TransactionID AND AT2007.OrderID = OT02.SOrderID)</t>
+      OR (AT2007.OTransactionID = OT02.TransactionID AND AT2007.OrderID = OT02.SOrderID)
+WHERE OT01.DivisionID = @DivisionID AND AT2007.VoucherID = @VoucherID</t>
+  </si>
+  <si>
+    <t>Nhận tham số từ màn hình AF0324 gọi màn hình AF0061 đồng thời thực thi @SQL0004 load dữ liệu lên màn hình AF0061 từ đơn hàng</t>
+  </si>
+  <si>
+    <t>@DivisionID @VoucherID</t>
+  </si>
+  <si>
+    <t>@@DivisionID @@VoucherID</t>
+  </si>
+  <si>
+    <t>@DivisionID, @VoucherID</t>
+  </si>
+  <si>
+    <t>- Customize cho Hoàng Trần (CustomizeIndex = 51): load đơn hàng theo barcode từ tham số truyền vào màn hình và cho phép kế thừa hóa đơn bán hàng</t>
+  </si>
+  <si>
+    <t>- Nhận tham số @DivisionID và @VoucherID gọi màn hình AF0061 và đồng thời thực thi @SQL0004 để load form AF0061</t>
   </si>
 </sst>
 </file>
@@ -2842,7 +2840,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="263">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3263,123 +3261,123 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3440,6 +3438,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3461,21 +3474,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3485,6 +3483,18 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3494,18 +3504,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3535,6 +3533,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -4467,65 +4468,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="183"/>
-      <c r="B1" s="183"/>
-      <c r="C1" s="185" t="s">
+      <c r="A1" s="177"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="179" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="184" t="s">
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="178" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184" t="s">
+      <c r="H1" s="178"/>
+      <c r="I1" s="178" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="184"/>
+      <c r="J1" s="178"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A2" s="183"/>
-      <c r="B2" s="183"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="184" t="s">
+      <c r="A2" s="177"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="178" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="178"/>
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A3" s="183"/>
-      <c r="B3" s="183"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="180" t="s">
+      <c r="A3" s="177"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="186"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="174" t="s">
         <v>160</v>
       </c>
-      <c r="H3" s="181"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="175"/>
     </row>
     <row r="4" spans="1:18">
       <c r="H4" s="113"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="182"/>
-      <c r="B13" s="182"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="182"/>
-      <c r="E13" s="182"/>
-      <c r="F13" s="182"/>
-      <c r="G13" s="182"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="182"/>
-      <c r="J13" s="182"/>
+      <c r="A13" s="176"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="176"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="176"/>
+      <c r="H13" s="176"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="176"/>
       <c r="K13" s="114"/>
       <c r="L13" s="114"/>
       <c r="M13" s="114"/>
@@ -4536,56 +4537,56 @@
       <c r="R13" s="114"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
-      <c r="B14" s="176"/>
-      <c r="C14" s="176"/>
-      <c r="D14" s="176"/>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
-      <c r="L14" s="176"/>
-      <c r="M14" s="176"/>
-      <c r="N14" s="176"/>
-      <c r="O14" s="176"/>
-      <c r="P14" s="176"/>
-      <c r="Q14" s="176"/>
-      <c r="R14" s="176"/>
+      <c r="B14" s="172"/>
+      <c r="C14" s="172"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="172"/>
+      <c r="F14" s="172"/>
+      <c r="G14" s="172"/>
+      <c r="H14" s="172"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="172"/>
+      <c r="M14" s="172"/>
+      <c r="N14" s="172"/>
+      <c r="O14" s="172"/>
+      <c r="P14" s="172"/>
+      <c r="Q14" s="172"/>
+      <c r="R14" s="172"/>
     </row>
     <row r="15" spans="1:18" ht="26.25">
-      <c r="B15" s="176"/>
-      <c r="C15" s="176"/>
-      <c r="D15" s="176"/>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
-      <c r="L15" s="176"/>
-      <c r="M15" s="176"/>
-      <c r="N15" s="176"/>
-      <c r="O15" s="176"/>
-      <c r="P15" s="176"/>
-      <c r="Q15" s="176"/>
-      <c r="R15" s="176"/>
+      <c r="B15" s="172"/>
+      <c r="C15" s="172"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="172"/>
+      <c r="F15" s="172"/>
+      <c r="G15" s="172"/>
+      <c r="H15" s="172"/>
+      <c r="I15" s="172"/>
+      <c r="J15" s="172"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="172"/>
+      <c r="M15" s="172"/>
+      <c r="N15" s="172"/>
+      <c r="O15" s="172"/>
+      <c r="P15" s="172"/>
+      <c r="Q15" s="172"/>
+      <c r="R15" s="172"/>
     </row>
     <row r="16" spans="1:18" ht="26.25">
-      <c r="A16" s="179" t="s">
+      <c r="A16" s="173" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="179"/>
-      <c r="C16" s="179"/>
-      <c r="D16" s="179"/>
-      <c r="E16" s="179"/>
-      <c r="F16" s="179"/>
-      <c r="G16" s="179"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="179"/>
-      <c r="J16" s="179"/>
+      <c r="B16" s="173"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="173"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
       <c r="K16" s="115"/>
       <c r="L16" s="115"/>
       <c r="M16" s="115"/>
@@ -4596,384 +4597,384 @@
       <c r="R16" s="115"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
-      <c r="B17" s="176"/>
-      <c r="C17" s="176"/>
-      <c r="D17" s="176"/>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="176"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="176"/>
-      <c r="P17" s="176"/>
-      <c r="Q17" s="176"/>
-      <c r="R17" s="176"/>
+      <c r="B17" s="172"/>
+      <c r="C17" s="172"/>
+      <c r="D17" s="172"/>
+      <c r="E17" s="172"/>
+      <c r="F17" s="172"/>
+      <c r="G17" s="172"/>
+      <c r="H17" s="172"/>
+      <c r="I17" s="172"/>
+      <c r="J17" s="172"/>
+      <c r="K17" s="172"/>
+      <c r="L17" s="172"/>
+      <c r="M17" s="172"/>
+      <c r="N17" s="172"/>
+      <c r="O17" s="172"/>
+      <c r="P17" s="172"/>
+      <c r="Q17" s="172"/>
+      <c r="R17" s="172"/>
     </row>
     <row r="18" spans="1:195" ht="26.25">
-      <c r="B18" s="176"/>
-      <c r="C18" s="176"/>
-      <c r="D18" s="176"/>
-      <c r="E18" s="176"/>
-      <c r="F18" s="176"/>
-      <c r="G18" s="176"/>
-      <c r="H18" s="176"/>
-      <c r="I18" s="176"/>
-      <c r="J18" s="176"/>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="176"/>
-      <c r="O18" s="176"/>
-      <c r="P18" s="176"/>
-      <c r="Q18" s="176"/>
-      <c r="R18" s="176"/>
+      <c r="B18" s="172"/>
+      <c r="C18" s="172"/>
+      <c r="D18" s="172"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
+      <c r="L18" s="172"/>
+      <c r="M18" s="172"/>
+      <c r="N18" s="172"/>
+      <c r="O18" s="172"/>
+      <c r="P18" s="172"/>
+      <c r="Q18" s="172"/>
+      <c r="R18" s="172"/>
     </row>
     <row r="19" spans="1:195" ht="23.25">
-      <c r="B19" s="178"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="178"/>
-      <c r="G19" s="178"/>
-      <c r="H19" s="178"/>
-      <c r="I19" s="178"/>
-      <c r="J19" s="178"/>
-      <c r="K19" s="178"/>
-      <c r="L19" s="178"/>
-      <c r="M19" s="178"/>
-      <c r="N19" s="178"/>
-      <c r="O19" s="178"/>
-      <c r="P19" s="178"/>
-      <c r="Q19" s="178"/>
-      <c r="R19" s="178"/>
+      <c r="B19" s="189"/>
+      <c r="C19" s="189"/>
+      <c r="D19" s="189"/>
+      <c r="E19" s="189"/>
+      <c r="F19" s="189"/>
+      <c r="G19" s="189"/>
+      <c r="H19" s="189"/>
+      <c r="I19" s="189"/>
+      <c r="J19" s="189"/>
+      <c r="K19" s="189"/>
+      <c r="L19" s="189"/>
+      <c r="M19" s="189"/>
+      <c r="N19" s="189"/>
+      <c r="O19" s="189"/>
+      <c r="P19" s="189"/>
+      <c r="Q19" s="189"/>
+      <c r="R19" s="189"/>
     </row>
     <row r="20" spans="1:195" ht="26.25">
-      <c r="B20" s="176"/>
-      <c r="C20" s="176"/>
-      <c r="D20" s="176"/>
-      <c r="E20" s="176"/>
-      <c r="F20" s="176"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176"/>
-      <c r="J20" s="176"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="176"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="176"/>
-      <c r="O20" s="176"/>
-      <c r="P20" s="176"/>
-      <c r="Q20" s="176"/>
-      <c r="R20" s="176"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="172"/>
+      <c r="I20" s="172"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
+      <c r="L20" s="172"/>
+      <c r="M20" s="172"/>
+      <c r="N20" s="172"/>
+      <c r="O20" s="172"/>
+      <c r="P20" s="172"/>
+      <c r="Q20" s="172"/>
+      <c r="R20" s="172"/>
     </row>
     <row r="21" spans="1:195" ht="26.25">
-      <c r="B21" s="176"/>
-      <c r="C21" s="176"/>
-      <c r="D21" s="176"/>
-      <c r="E21" s="176"/>
-      <c r="F21" s="176"/>
-      <c r="G21" s="176"/>
-      <c r="H21" s="176"/>
-      <c r="I21" s="176"/>
-      <c r="J21" s="176"/>
-      <c r="K21" s="176"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="176"/>
-      <c r="O21" s="176"/>
-      <c r="P21" s="176"/>
-      <c r="Q21" s="176"/>
-      <c r="R21" s="176"/>
+      <c r="B21" s="172"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="172"/>
+      <c r="G21" s="172"/>
+      <c r="H21" s="172"/>
+      <c r="I21" s="172"/>
+      <c r="J21" s="172"/>
+      <c r="K21" s="172"/>
+      <c r="L21" s="172"/>
+      <c r="M21" s="172"/>
+      <c r="N21" s="172"/>
+      <c r="O21" s="172"/>
+      <c r="P21" s="172"/>
+      <c r="Q21" s="172"/>
+      <c r="R21" s="172"/>
     </row>
     <row r="22" spans="1:195" ht="25.5">
-      <c r="B22" s="177"/>
-      <c r="C22" s="177"/>
-      <c r="D22" s="177"/>
-      <c r="E22" s="177"/>
-      <c r="F22" s="177"/>
-      <c r="G22" s="177"/>
-      <c r="H22" s="177"/>
-      <c r="I22" s="177"/>
-      <c r="J22" s="177"/>
-      <c r="K22" s="177"/>
-      <c r="L22" s="177"/>
-      <c r="M22" s="177"/>
-      <c r="N22" s="177"/>
-      <c r="O22" s="177"/>
-      <c r="P22" s="177"/>
-      <c r="Q22" s="177"/>
-      <c r="R22" s="177"/>
+      <c r="B22" s="188"/>
+      <c r="C22" s="188"/>
+      <c r="D22" s="188"/>
+      <c r="E22" s="188"/>
+      <c r="F22" s="188"/>
+      <c r="G22" s="188"/>
+      <c r="H22" s="188"/>
+      <c r="I22" s="188"/>
+      <c r="J22" s="188"/>
+      <c r="K22" s="188"/>
+      <c r="L22" s="188"/>
+      <c r="M22" s="188"/>
+      <c r="N22" s="188"/>
+      <c r="O22" s="188"/>
+      <c r="P22" s="188"/>
+      <c r="Q22" s="188"/>
+      <c r="R22" s="188"/>
     </row>
     <row r="23" spans="1:195" ht="25.5">
-      <c r="B23" s="177"/>
-      <c r="C23" s="177"/>
-      <c r="D23" s="177"/>
-      <c r="E23" s="177"/>
-      <c r="F23" s="177"/>
-      <c r="G23" s="177"/>
-      <c r="H23" s="177"/>
-      <c r="I23" s="177"/>
-      <c r="J23" s="177"/>
-      <c r="K23" s="177"/>
-      <c r="L23" s="177"/>
-      <c r="M23" s="177"/>
-      <c r="N23" s="177"/>
-      <c r="O23" s="177"/>
-      <c r="P23" s="177"/>
-      <c r="Q23" s="177"/>
-      <c r="R23" s="177"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="188"/>
+      <c r="D23" s="188"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="188"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
+      <c r="K23" s="188"/>
+      <c r="L23" s="188"/>
+      <c r="M23" s="188"/>
+      <c r="N23" s="188"/>
+      <c r="O23" s="188"/>
+      <c r="P23" s="188"/>
+      <c r="Q23" s="188"/>
+      <c r="R23" s="188"/>
     </row>
     <row r="25" spans="1:195" ht="11.25" customHeight="1"/>
     <row r="26" spans="1:195" ht="18">
-      <c r="B26" s="174"/>
-      <c r="C26" s="174"/>
-      <c r="D26" s="174"/>
-      <c r="E26" s="174"/>
-      <c r="F26" s="174"/>
-      <c r="G26" s="174"/>
-      <c r="H26" s="174"/>
-      <c r="I26" s="174"/>
-      <c r="J26" s="174"/>
-      <c r="K26" s="174"/>
-      <c r="L26" s="174"/>
-      <c r="M26" s="174"/>
-      <c r="N26" s="174"/>
-      <c r="O26" s="174"/>
-      <c r="P26" s="174"/>
-      <c r="Q26" s="174"/>
-      <c r="R26" s="174"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="190"/>
+      <c r="D26" s="190"/>
+      <c r="E26" s="190"/>
+      <c r="F26" s="190"/>
+      <c r="G26" s="190"/>
+      <c r="H26" s="190"/>
+      <c r="I26" s="190"/>
+      <c r="J26" s="190"/>
+      <c r="K26" s="190"/>
+      <c r="L26" s="190"/>
+      <c r="M26" s="190"/>
+      <c r="N26" s="190"/>
+      <c r="O26" s="190"/>
+      <c r="P26" s="190"/>
+      <c r="Q26" s="190"/>
+      <c r="R26" s="190"/>
     </row>
     <row r="28" spans="1:195" ht="18">
-      <c r="B28" s="175"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="175"/>
-      <c r="E28" s="175"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="175"/>
-      <c r="H28" s="175"/>
-      <c r="I28" s="175"/>
-      <c r="J28" s="175"/>
-      <c r="K28" s="175"/>
-      <c r="L28" s="175"/>
-      <c r="M28" s="175"/>
-      <c r="N28" s="175"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="175"/>
-      <c r="Q28" s="175"/>
-      <c r="R28" s="175"/>
-      <c r="S28" s="173"/>
-      <c r="T28" s="173"/>
-      <c r="U28" s="173"/>
-      <c r="V28" s="173"/>
-      <c r="W28" s="173"/>
-      <c r="X28" s="173"/>
-      <c r="Y28" s="173"/>
-      <c r="Z28" s="173"/>
-      <c r="AA28" s="173"/>
-      <c r="AB28" s="173"/>
-      <c r="AC28" s="173"/>
-      <c r="AD28" s="173"/>
-      <c r="AE28" s="173"/>
-      <c r="AF28" s="173"/>
-      <c r="AG28" s="173"/>
-      <c r="AH28" s="173"/>
-      <c r="AI28" s="173"/>
-      <c r="AJ28" s="173"/>
-      <c r="AK28" s="173"/>
-      <c r="AL28" s="173"/>
-      <c r="AM28" s="173"/>
-      <c r="AN28" s="173"/>
-      <c r="AO28" s="173"/>
-      <c r="AP28" s="173"/>
-      <c r="AQ28" s="173"/>
-      <c r="AR28" s="173"/>
-      <c r="AS28" s="173"/>
-      <c r="AT28" s="173"/>
-      <c r="AU28" s="173"/>
-      <c r="AV28" s="173"/>
-      <c r="AW28" s="173"/>
-      <c r="AX28" s="173"/>
-      <c r="AY28" s="173"/>
-      <c r="AZ28" s="173"/>
-      <c r="BA28" s="173"/>
-      <c r="BB28" s="173"/>
-      <c r="BC28" s="173"/>
-      <c r="BD28" s="173"/>
-      <c r="BE28" s="173"/>
-      <c r="BF28" s="173"/>
-      <c r="BG28" s="173"/>
-      <c r="BH28" s="173"/>
-      <c r="BI28" s="173"/>
-      <c r="BJ28" s="173"/>
-      <c r="BK28" s="173"/>
-      <c r="BL28" s="173"/>
-      <c r="BM28" s="173"/>
-      <c r="BN28" s="173"/>
-      <c r="BO28" s="173"/>
-      <c r="BP28" s="173"/>
-      <c r="BQ28" s="173"/>
-      <c r="BR28" s="173"/>
-      <c r="BS28" s="173"/>
-      <c r="BT28" s="173"/>
-      <c r="BU28" s="173"/>
-      <c r="BV28" s="173"/>
-      <c r="BW28" s="173"/>
-      <c r="BX28" s="173"/>
-      <c r="BY28" s="173"/>
-      <c r="BZ28" s="173"/>
-      <c r="CA28" s="173"/>
-      <c r="CB28" s="173"/>
-      <c r="CC28" s="173"/>
-      <c r="CD28" s="173"/>
-      <c r="CE28" s="173"/>
-      <c r="CF28" s="173"/>
-      <c r="CG28" s="173"/>
-      <c r="CH28" s="173"/>
-      <c r="CI28" s="173"/>
-      <c r="CJ28" s="173"/>
-      <c r="CK28" s="173"/>
-      <c r="CL28" s="173"/>
-      <c r="CM28" s="173"/>
-      <c r="CN28" s="173"/>
-      <c r="CO28" s="173"/>
-      <c r="CP28" s="173"/>
-      <c r="CQ28" s="173"/>
-      <c r="CR28" s="173"/>
-      <c r="CS28" s="173"/>
-      <c r="CT28" s="173"/>
-      <c r="CU28" s="173"/>
-      <c r="CV28" s="173"/>
-      <c r="CW28" s="173"/>
-      <c r="CX28" s="173"/>
-      <c r="CY28" s="173"/>
-      <c r="CZ28" s="173"/>
-      <c r="DA28" s="173"/>
-      <c r="DB28" s="173"/>
-      <c r="DC28" s="173"/>
-      <c r="DD28" s="173"/>
-      <c r="DE28" s="173"/>
-      <c r="DF28" s="173"/>
-      <c r="DG28" s="173"/>
-      <c r="DH28" s="173"/>
-      <c r="DI28" s="173"/>
-      <c r="DJ28" s="173"/>
-      <c r="DK28" s="173"/>
-      <c r="DL28" s="173"/>
-      <c r="DM28" s="173"/>
-      <c r="DN28" s="173"/>
-      <c r="DO28" s="173"/>
-      <c r="DP28" s="173"/>
-      <c r="DQ28" s="173"/>
-      <c r="DR28" s="173"/>
-      <c r="DS28" s="173"/>
-      <c r="DT28" s="173"/>
-      <c r="DU28" s="173"/>
-      <c r="DV28" s="173"/>
-      <c r="DW28" s="173"/>
-      <c r="DX28" s="173"/>
-      <c r="DY28" s="173"/>
-      <c r="DZ28" s="173"/>
-      <c r="EA28" s="173"/>
-      <c r="EB28" s="173"/>
-      <c r="EC28" s="173"/>
-      <c r="ED28" s="173"/>
-      <c r="EE28" s="173"/>
-      <c r="EF28" s="173"/>
-      <c r="EG28" s="173"/>
-      <c r="EH28" s="173"/>
-      <c r="EI28" s="173"/>
-      <c r="EJ28" s="173"/>
-      <c r="EK28" s="173"/>
-      <c r="EL28" s="173"/>
-      <c r="EM28" s="173"/>
-      <c r="EN28" s="173"/>
-      <c r="EO28" s="173"/>
-      <c r="EP28" s="173"/>
-      <c r="EQ28" s="173"/>
-      <c r="ER28" s="173"/>
-      <c r="ES28" s="173"/>
-      <c r="ET28" s="173"/>
-      <c r="EU28" s="173"/>
-      <c r="EV28" s="173"/>
-      <c r="EW28" s="173"/>
-      <c r="EX28" s="173"/>
-      <c r="EY28" s="173"/>
-      <c r="EZ28" s="173"/>
-      <c r="FA28" s="173"/>
-      <c r="FB28" s="173"/>
-      <c r="FC28" s="173"/>
-      <c r="FD28" s="173"/>
-      <c r="FE28" s="173"/>
-      <c r="FF28" s="173"/>
-      <c r="FG28" s="173"/>
-      <c r="FH28" s="173"/>
-      <c r="FI28" s="173"/>
-      <c r="FJ28" s="173"/>
-      <c r="FK28" s="173"/>
-      <c r="FL28" s="173"/>
-      <c r="FM28" s="173"/>
-      <c r="FN28" s="173"/>
-      <c r="FO28" s="173"/>
-      <c r="FP28" s="173"/>
-      <c r="FQ28" s="173"/>
-      <c r="FR28" s="173"/>
-      <c r="FS28" s="173"/>
-      <c r="FT28" s="173"/>
-      <c r="FU28" s="173"/>
-      <c r="FV28" s="173"/>
-      <c r="FW28" s="173"/>
-      <c r="FX28" s="173"/>
-      <c r="FY28" s="173"/>
-      <c r="FZ28" s="173"/>
-      <c r="GA28" s="173"/>
-      <c r="GB28" s="173"/>
-      <c r="GC28" s="173"/>
-      <c r="GD28" s="173"/>
-      <c r="GE28" s="173"/>
-      <c r="GF28" s="173"/>
-      <c r="GG28" s="173"/>
-      <c r="GH28" s="173"/>
-      <c r="GI28" s="173"/>
-      <c r="GJ28" s="173"/>
-      <c r="GK28" s="173"/>
-      <c r="GL28" s="173"/>
+      <c r="B28" s="192"/>
+      <c r="C28" s="192"/>
+      <c r="D28" s="192"/>
+      <c r="E28" s="192"/>
+      <c r="F28" s="192"/>
+      <c r="G28" s="192"/>
+      <c r="H28" s="192"/>
+      <c r="I28" s="192"/>
+      <c r="J28" s="192"/>
+      <c r="K28" s="192"/>
+      <c r="L28" s="192"/>
+      <c r="M28" s="192"/>
+      <c r="N28" s="192"/>
+      <c r="O28" s="192"/>
+      <c r="P28" s="192"/>
+      <c r="Q28" s="192"/>
+      <c r="R28" s="192"/>
+      <c r="S28" s="191"/>
+      <c r="T28" s="191"/>
+      <c r="U28" s="191"/>
+      <c r="V28" s="191"/>
+      <c r="W28" s="191"/>
+      <c r="X28" s="191"/>
+      <c r="Y28" s="191"/>
+      <c r="Z28" s="191"/>
+      <c r="AA28" s="191"/>
+      <c r="AB28" s="191"/>
+      <c r="AC28" s="191"/>
+      <c r="AD28" s="191"/>
+      <c r="AE28" s="191"/>
+      <c r="AF28" s="191"/>
+      <c r="AG28" s="191"/>
+      <c r="AH28" s="191"/>
+      <c r="AI28" s="191"/>
+      <c r="AJ28" s="191"/>
+      <c r="AK28" s="191"/>
+      <c r="AL28" s="191"/>
+      <c r="AM28" s="191"/>
+      <c r="AN28" s="191"/>
+      <c r="AO28" s="191"/>
+      <c r="AP28" s="191"/>
+      <c r="AQ28" s="191"/>
+      <c r="AR28" s="191"/>
+      <c r="AS28" s="191"/>
+      <c r="AT28" s="191"/>
+      <c r="AU28" s="191"/>
+      <c r="AV28" s="191"/>
+      <c r="AW28" s="191"/>
+      <c r="AX28" s="191"/>
+      <c r="AY28" s="191"/>
+      <c r="AZ28" s="191"/>
+      <c r="BA28" s="191"/>
+      <c r="BB28" s="191"/>
+      <c r="BC28" s="191"/>
+      <c r="BD28" s="191"/>
+      <c r="BE28" s="191"/>
+      <c r="BF28" s="191"/>
+      <c r="BG28" s="191"/>
+      <c r="BH28" s="191"/>
+      <c r="BI28" s="191"/>
+      <c r="BJ28" s="191"/>
+      <c r="BK28" s="191"/>
+      <c r="BL28" s="191"/>
+      <c r="BM28" s="191"/>
+      <c r="BN28" s="191"/>
+      <c r="BO28" s="191"/>
+      <c r="BP28" s="191"/>
+      <c r="BQ28" s="191"/>
+      <c r="BR28" s="191"/>
+      <c r="BS28" s="191"/>
+      <c r="BT28" s="191"/>
+      <c r="BU28" s="191"/>
+      <c r="BV28" s="191"/>
+      <c r="BW28" s="191"/>
+      <c r="BX28" s="191"/>
+      <c r="BY28" s="191"/>
+      <c r="BZ28" s="191"/>
+      <c r="CA28" s="191"/>
+      <c r="CB28" s="191"/>
+      <c r="CC28" s="191"/>
+      <c r="CD28" s="191"/>
+      <c r="CE28" s="191"/>
+      <c r="CF28" s="191"/>
+      <c r="CG28" s="191"/>
+      <c r="CH28" s="191"/>
+      <c r="CI28" s="191"/>
+      <c r="CJ28" s="191"/>
+      <c r="CK28" s="191"/>
+      <c r="CL28" s="191"/>
+      <c r="CM28" s="191"/>
+      <c r="CN28" s="191"/>
+      <c r="CO28" s="191"/>
+      <c r="CP28" s="191"/>
+      <c r="CQ28" s="191"/>
+      <c r="CR28" s="191"/>
+      <c r="CS28" s="191"/>
+      <c r="CT28" s="191"/>
+      <c r="CU28" s="191"/>
+      <c r="CV28" s="191"/>
+      <c r="CW28" s="191"/>
+      <c r="CX28" s="191"/>
+      <c r="CY28" s="191"/>
+      <c r="CZ28" s="191"/>
+      <c r="DA28" s="191"/>
+      <c r="DB28" s="191"/>
+      <c r="DC28" s="191"/>
+      <c r="DD28" s="191"/>
+      <c r="DE28" s="191"/>
+      <c r="DF28" s="191"/>
+      <c r="DG28" s="191"/>
+      <c r="DH28" s="191"/>
+      <c r="DI28" s="191"/>
+      <c r="DJ28" s="191"/>
+      <c r="DK28" s="191"/>
+      <c r="DL28" s="191"/>
+      <c r="DM28" s="191"/>
+      <c r="DN28" s="191"/>
+      <c r="DO28" s="191"/>
+      <c r="DP28" s="191"/>
+      <c r="DQ28" s="191"/>
+      <c r="DR28" s="191"/>
+      <c r="DS28" s="191"/>
+      <c r="DT28" s="191"/>
+      <c r="DU28" s="191"/>
+      <c r="DV28" s="191"/>
+      <c r="DW28" s="191"/>
+      <c r="DX28" s="191"/>
+      <c r="DY28" s="191"/>
+      <c r="DZ28" s="191"/>
+      <c r="EA28" s="191"/>
+      <c r="EB28" s="191"/>
+      <c r="EC28" s="191"/>
+      <c r="ED28" s="191"/>
+      <c r="EE28" s="191"/>
+      <c r="EF28" s="191"/>
+      <c r="EG28" s="191"/>
+      <c r="EH28" s="191"/>
+      <c r="EI28" s="191"/>
+      <c r="EJ28" s="191"/>
+      <c r="EK28" s="191"/>
+      <c r="EL28" s="191"/>
+      <c r="EM28" s="191"/>
+      <c r="EN28" s="191"/>
+      <c r="EO28" s="191"/>
+      <c r="EP28" s="191"/>
+      <c r="EQ28" s="191"/>
+      <c r="ER28" s="191"/>
+      <c r="ES28" s="191"/>
+      <c r="ET28" s="191"/>
+      <c r="EU28" s="191"/>
+      <c r="EV28" s="191"/>
+      <c r="EW28" s="191"/>
+      <c r="EX28" s="191"/>
+      <c r="EY28" s="191"/>
+      <c r="EZ28" s="191"/>
+      <c r="FA28" s="191"/>
+      <c r="FB28" s="191"/>
+      <c r="FC28" s="191"/>
+      <c r="FD28" s="191"/>
+      <c r="FE28" s="191"/>
+      <c r="FF28" s="191"/>
+      <c r="FG28" s="191"/>
+      <c r="FH28" s="191"/>
+      <c r="FI28" s="191"/>
+      <c r="FJ28" s="191"/>
+      <c r="FK28" s="191"/>
+      <c r="FL28" s="191"/>
+      <c r="FM28" s="191"/>
+      <c r="FN28" s="191"/>
+      <c r="FO28" s="191"/>
+      <c r="FP28" s="191"/>
+      <c r="FQ28" s="191"/>
+      <c r="FR28" s="191"/>
+      <c r="FS28" s="191"/>
+      <c r="FT28" s="191"/>
+      <c r="FU28" s="191"/>
+      <c r="FV28" s="191"/>
+      <c r="FW28" s="191"/>
+      <c r="FX28" s="191"/>
+      <c r="FY28" s="191"/>
+      <c r="FZ28" s="191"/>
+      <c r="GA28" s="191"/>
+      <c r="GB28" s="191"/>
+      <c r="GC28" s="191"/>
+      <c r="GD28" s="191"/>
+      <c r="GE28" s="191"/>
+      <c r="GF28" s="191"/>
+      <c r="GG28" s="191"/>
+      <c r="GH28" s="191"/>
+      <c r="GI28" s="191"/>
+      <c r="GJ28" s="191"/>
+      <c r="GK28" s="191"/>
+      <c r="GL28" s="191"/>
       <c r="GM28" s="116"/>
     </row>
     <row r="29" spans="1:195" ht="18">
-      <c r="B29" s="174"/>
-      <c r="C29" s="174"/>
-      <c r="D29" s="174"/>
-      <c r="E29" s="174"/>
-      <c r="F29" s="174"/>
-      <c r="G29" s="174"/>
-      <c r="H29" s="174"/>
-      <c r="I29" s="174"/>
-      <c r="J29" s="174"/>
-      <c r="K29" s="174"/>
-      <c r="L29" s="174"/>
-      <c r="M29" s="174"/>
-      <c r="N29" s="174"/>
-      <c r="O29" s="174"/>
-      <c r="P29" s="174"/>
-      <c r="Q29" s="174"/>
-      <c r="R29" s="174"/>
+      <c r="B29" s="190"/>
+      <c r="C29" s="190"/>
+      <c r="D29" s="190"/>
+      <c r="E29" s="190"/>
+      <c r="F29" s="190"/>
+      <c r="G29" s="190"/>
+      <c r="H29" s="190"/>
+      <c r="I29" s="190"/>
+      <c r="J29" s="190"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
+      <c r="M29" s="190"/>
+      <c r="N29" s="190"/>
+      <c r="O29" s="190"/>
+      <c r="P29" s="190"/>
+      <c r="Q29" s="190"/>
+      <c r="R29" s="190"/>
     </row>
     <row r="30" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A30" s="172"/>
-      <c r="B30" s="172"/>
-      <c r="C30" s="172"/>
-      <c r="D30" s="172"/>
-      <c r="E30" s="172"/>
-      <c r="F30" s="172"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="172"/>
+      <c r="A30" s="193"/>
+      <c r="B30" s="193"/>
+      <c r="C30" s="193"/>
+      <c r="D30" s="193"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
       <c r="K30" s="117"/>
       <c r="L30" s="117"/>
       <c r="M30" s="117"/>
@@ -4984,16 +4985,16 @@
       <c r="R30" s="117"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A31" s="172"/>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
-      <c r="D31" s="172"/>
-      <c r="E31" s="172"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="172"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="172"/>
-      <c r="J31" s="172"/>
+      <c r="A31" s="193"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="193"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
       <c r="K31" s="117"/>
       <c r="L31" s="117"/>
       <c r="M31" s="117"/>
@@ -5005,6 +5006,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="DF28:DV28"/>
+    <mergeCell ref="DW28:EM28"/>
+    <mergeCell ref="EN28:FD28"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="FE28:FU28"/>
+    <mergeCell ref="FV28:GL28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="Y28:AO28"/>
+    <mergeCell ref="AP28:BF28"/>
+    <mergeCell ref="BG28:BW28"/>
+    <mergeCell ref="BX28:CN28"/>
+    <mergeCell ref="CO28:DE28"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B19:R19"/>
     <mergeCell ref="B14:R14"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="A16:J16"/>
@@ -5018,28 +5041,6 @@
     <mergeCell ref="C1:F3"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="FE28:FU28"/>
-    <mergeCell ref="FV28:GL28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="S28:X28"/>
-    <mergeCell ref="Y28:AO28"/>
-    <mergeCell ref="AP28:BF28"/>
-    <mergeCell ref="BG28:BW28"/>
-    <mergeCell ref="BX28:CN28"/>
-    <mergeCell ref="CO28:DE28"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="DF28:DV28"/>
-    <mergeCell ref="DW28:EM28"/>
-    <mergeCell ref="EN28:FD28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>
@@ -5578,7 +5579,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J2"/>
+      <selection activeCell="E7" sqref="E7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -5594,10 +5595,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -5624,8 +5625,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5664,14 +5665,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="205" t="s">
+      <c r="E4" s="204" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="205"/>
-      <c r="G4" s="205"/>
-      <c r="H4" s="205"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205"/>
+      <c r="F4" s="204"/>
+      <c r="G4" s="204"/>
+      <c r="H4" s="204"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5" s="40">
@@ -5686,14 +5687,14 @@
       <c r="D5" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="206" t="s">
+      <c r="E5" s="205" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="207"/>
-      <c r="G5" s="207"/>
-      <c r="H5" s="207"/>
-      <c r="I5" s="207"/>
-      <c r="J5" s="207"/>
+      <c r="F5" s="206"/>
+      <c r="G5" s="206"/>
+      <c r="H5" s="206"/>
+      <c r="I5" s="206"/>
+      <c r="J5" s="206"/>
     </row>
     <row r="6" spans="1:10" s="127" customFormat="1" ht="25.5" customHeight="1">
       <c r="A6" s="128">
@@ -5708,14 +5709,14 @@
       <c r="D6" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="208" t="s">
+      <c r="E6" s="207" t="s">
         <v>192</v>
       </c>
-      <c r="F6" s="209"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="209"/>
-      <c r="I6" s="209"/>
-      <c r="J6" s="210"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="208"/>
+      <c r="H6" s="208"/>
+      <c r="I6" s="208"/>
+      <c r="J6" s="209"/>
     </row>
     <row r="7" spans="1:10" s="151" customFormat="1" ht="24.75" customHeight="1">
       <c r="A7" s="88">
@@ -5730,14 +5731,14 @@
       <c r="D7" s="150" t="s">
         <v>208</v>
       </c>
-      <c r="E7" s="198" t="s">
-        <v>225</v>
-      </c>
-      <c r="F7" s="199"/>
-      <c r="G7" s="199"/>
-      <c r="H7" s="199"/>
-      <c r="I7" s="199"/>
-      <c r="J7" s="200"/>
+      <c r="E7" s="194" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="195"/>
+      <c r="G7" s="195"/>
+      <c r="H7" s="195"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="196"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="89">
@@ -5748,12 +5749,12 @@
       </c>
       <c r="C8" s="75"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="201"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="202"/>
-      <c r="H8" s="202"/>
-      <c r="I8" s="202"/>
-      <c r="J8" s="203"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="198"/>
+      <c r="G8" s="198"/>
+      <c r="H8" s="198"/>
+      <c r="I8" s="198"/>
+      <c r="J8" s="199"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="90">
@@ -5764,12 +5765,12 @@
       </c>
       <c r="C9" s="75"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="195"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="196"/>
-      <c r="I9" s="196"/>
-      <c r="J9" s="197"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="202"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="91">
@@ -5780,12 +5781,12 @@
       </c>
       <c r="C10" s="75"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="195"/>
-      <c r="F10" s="196"/>
-      <c r="G10" s="196"/>
-      <c r="H10" s="196"/>
-      <c r="I10" s="196"/>
-      <c r="J10" s="197"/>
+      <c r="E10" s="200"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="201"/>
+      <c r="J10" s="202"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="92">
@@ -5796,12 +5797,12 @@
       </c>
       <c r="C11" s="75"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="195"/>
-      <c r="F11" s="196"/>
-      <c r="G11" s="196"/>
-      <c r="H11" s="196"/>
-      <c r="I11" s="196"/>
-      <c r="J11" s="197"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="202"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="93">
@@ -5812,12 +5813,12 @@
       </c>
       <c r="C12" s="75"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="195"/>
-      <c r="F12" s="196"/>
-      <c r="G12" s="196"/>
-      <c r="H12" s="196"/>
-      <c r="I12" s="196"/>
-      <c r="J12" s="197"/>
+      <c r="E12" s="200"/>
+      <c r="F12" s="201"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="201"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="202"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="94">
@@ -5828,12 +5829,12 @@
       </c>
       <c r="C13" s="75"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="195"/>
-      <c r="F13" s="196"/>
-      <c r="G13" s="196"/>
-      <c r="H13" s="196"/>
-      <c r="I13" s="196"/>
-      <c r="J13" s="197"/>
+      <c r="E13" s="200"/>
+      <c r="F13" s="201"/>
+      <c r="G13" s="201"/>
+      <c r="H13" s="201"/>
+      <c r="I13" s="201"/>
+      <c r="J13" s="202"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="95">
@@ -5844,12 +5845,12 @@
       </c>
       <c r="C14" s="75"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="195"/>
-      <c r="F14" s="196"/>
-      <c r="G14" s="196"/>
-      <c r="H14" s="196"/>
-      <c r="I14" s="196"/>
-      <c r="J14" s="197"/>
+      <c r="E14" s="200"/>
+      <c r="F14" s="201"/>
+      <c r="G14" s="201"/>
+      <c r="H14" s="201"/>
+      <c r="I14" s="201"/>
+      <c r="J14" s="202"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="40">
@@ -5860,12 +5861,12 @@
       </c>
       <c r="C15" s="75"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="194"/>
-      <c r="F15" s="194"/>
-      <c r="G15" s="194"/>
-      <c r="H15" s="194"/>
-      <c r="I15" s="194"/>
-      <c r="J15" s="194"/>
+      <c r="E15" s="210"/>
+      <c r="F15" s="210"/>
+      <c r="G15" s="210"/>
+      <c r="H15" s="210"/>
+      <c r="I15" s="210"/>
+      <c r="J15" s="210"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="87">
@@ -5876,12 +5877,12 @@
       </c>
       <c r="C16" s="75"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="194"/>
-      <c r="F16" s="194"/>
-      <c r="G16" s="194"/>
-      <c r="H16" s="194"/>
-      <c r="I16" s="194"/>
-      <c r="J16" s="194"/>
+      <c r="E16" s="210"/>
+      <c r="F16" s="210"/>
+      <c r="G16" s="210"/>
+      <c r="H16" s="210"/>
+      <c r="I16" s="210"/>
+      <c r="J16" s="210"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="88">
@@ -5892,12 +5893,12 @@
       </c>
       <c r="C17" s="75"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="194"/>
-      <c r="F17" s="194"/>
-      <c r="G17" s="194"/>
-      <c r="H17" s="194"/>
-      <c r="I17" s="194"/>
-      <c r="J17" s="194"/>
+      <c r="E17" s="210"/>
+      <c r="F17" s="210"/>
+      <c r="G17" s="210"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="210"/>
+      <c r="J17" s="210"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="89">
@@ -5908,12 +5909,12 @@
       </c>
       <c r="C18" s="75"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="194"/>
-      <c r="F18" s="194"/>
-      <c r="G18" s="194"/>
-      <c r="H18" s="194"/>
-      <c r="I18" s="194"/>
-      <c r="J18" s="194"/>
+      <c r="E18" s="210"/>
+      <c r="F18" s="210"/>
+      <c r="G18" s="210"/>
+      <c r="H18" s="210"/>
+      <c r="I18" s="210"/>
+      <c r="J18" s="210"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="90">
@@ -5924,12 +5925,12 @@
       </c>
       <c r="C19" s="75"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="194"/>
-      <c r="F19" s="194"/>
-      <c r="G19" s="194"/>
-      <c r="H19" s="194"/>
-      <c r="I19" s="194"/>
-      <c r="J19" s="194"/>
+      <c r="E19" s="210"/>
+      <c r="F19" s="210"/>
+      <c r="G19" s="210"/>
+      <c r="H19" s="210"/>
+      <c r="I19" s="210"/>
+      <c r="J19" s="210"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="91">
@@ -5940,12 +5941,12 @@
       </c>
       <c r="C20" s="75"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="194"/>
-      <c r="F20" s="194"/>
-      <c r="G20" s="194"/>
-      <c r="H20" s="194"/>
-      <c r="I20" s="194"/>
-      <c r="J20" s="194"/>
+      <c r="E20" s="210"/>
+      <c r="F20" s="210"/>
+      <c r="G20" s="210"/>
+      <c r="H20" s="210"/>
+      <c r="I20" s="210"/>
+      <c r="J20" s="210"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="92">
@@ -5956,12 +5957,12 @@
       </c>
       <c r="C21" s="75"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="194"/>
+      <c r="E21" s="210"/>
+      <c r="F21" s="210"/>
+      <c r="G21" s="210"/>
+      <c r="H21" s="210"/>
+      <c r="I21" s="210"/>
+      <c r="J21" s="210"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="93">
@@ -5972,12 +5973,12 @@
       </c>
       <c r="C22" s="75"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="194"/>
-      <c r="F22" s="194"/>
-      <c r="G22" s="194"/>
-      <c r="H22" s="194"/>
-      <c r="I22" s="194"/>
-      <c r="J22" s="194"/>
+      <c r="E22" s="210"/>
+      <c r="F22" s="210"/>
+      <c r="G22" s="210"/>
+      <c r="H22" s="210"/>
+      <c r="I22" s="210"/>
+      <c r="J22" s="210"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="94">
@@ -5988,12 +5989,12 @@
       </c>
       <c r="C23" s="75"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="194"/>
-      <c r="F23" s="194"/>
-      <c r="G23" s="194"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="194"/>
-      <c r="J23" s="194"/>
+      <c r="E23" s="210"/>
+      <c r="F23" s="210"/>
+      <c r="G23" s="210"/>
+      <c r="H23" s="210"/>
+      <c r="I23" s="210"/>
+      <c r="J23" s="210"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="95">
@@ -6004,12 +6005,12 @@
       </c>
       <c r="C24" s="75"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="194"/>
-      <c r="F24" s="194"/>
-      <c r="G24" s="194"/>
-      <c r="H24" s="194"/>
-      <c r="I24" s="194"/>
-      <c r="J24" s="194"/>
+      <c r="E24" s="210"/>
+      <c r="F24" s="210"/>
+      <c r="G24" s="210"/>
+      <c r="H24" s="210"/>
+      <c r="I24" s="210"/>
+      <c r="J24" s="210"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="40">
@@ -6020,12 +6021,12 @@
       </c>
       <c r="C25" s="75"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
-      <c r="J25" s="194"/>
+      <c r="E25" s="210"/>
+      <c r="F25" s="210"/>
+      <c r="G25" s="210"/>
+      <c r="H25" s="210"/>
+      <c r="I25" s="210"/>
+      <c r="J25" s="210"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="40">
@@ -6036,12 +6037,12 @@
       </c>
       <c r="C26" s="75"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="194"/>
-      <c r="F26" s="194"/>
-      <c r="G26" s="194"/>
-      <c r="H26" s="194"/>
-      <c r="I26" s="194"/>
-      <c r="J26" s="194"/>
+      <c r="E26" s="210"/>
+      <c r="F26" s="210"/>
+      <c r="G26" s="210"/>
+      <c r="H26" s="210"/>
+      <c r="I26" s="210"/>
+      <c r="J26" s="210"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="87">
@@ -6052,12 +6053,12 @@
       </c>
       <c r="C27" s="75"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="194"/>
-      <c r="F27" s="194"/>
-      <c r="G27" s="194"/>
-      <c r="H27" s="194"/>
-      <c r="I27" s="194"/>
-      <c r="J27" s="194"/>
+      <c r="E27" s="210"/>
+      <c r="F27" s="210"/>
+      <c r="G27" s="210"/>
+      <c r="H27" s="210"/>
+      <c r="I27" s="210"/>
+      <c r="J27" s="210"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="88">
@@ -6068,12 +6069,12 @@
       </c>
       <c r="C28" s="75"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="194"/>
-      <c r="F28" s="194"/>
-      <c r="G28" s="194"/>
-      <c r="H28" s="194"/>
-      <c r="I28" s="194"/>
-      <c r="J28" s="194"/>
+      <c r="E28" s="210"/>
+      <c r="F28" s="210"/>
+      <c r="G28" s="210"/>
+      <c r="H28" s="210"/>
+      <c r="I28" s="210"/>
+      <c r="J28" s="210"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="89">
@@ -6084,12 +6085,12 @@
       </c>
       <c r="C29" s="75"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="194"/>
-      <c r="F29" s="194"/>
-      <c r="G29" s="194"/>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="194"/>
+      <c r="E29" s="210"/>
+      <c r="F29" s="210"/>
+      <c r="G29" s="210"/>
+      <c r="H29" s="210"/>
+      <c r="I29" s="210"/>
+      <c r="J29" s="210"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="90">
@@ -6100,12 +6101,12 @@
       </c>
       <c r="C30" s="75"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="194"/>
-      <c r="F30" s="194"/>
-      <c r="G30" s="194"/>
-      <c r="H30" s="194"/>
-      <c r="I30" s="194"/>
-      <c r="J30" s="194"/>
+      <c r="E30" s="210"/>
+      <c r="F30" s="210"/>
+      <c r="G30" s="210"/>
+      <c r="H30" s="210"/>
+      <c r="I30" s="210"/>
+      <c r="J30" s="210"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="91">
@@ -6116,12 +6117,12 @@
       </c>
       <c r="C31" s="75"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="194"/>
-      <c r="F31" s="194"/>
-      <c r="G31" s="194"/>
-      <c r="H31" s="194"/>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
+      <c r="E31" s="210"/>
+      <c r="F31" s="210"/>
+      <c r="G31" s="210"/>
+      <c r="H31" s="210"/>
+      <c r="I31" s="210"/>
+      <c r="J31" s="210"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="92">
@@ -6132,12 +6133,12 @@
       </c>
       <c r="C32" s="75"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="194"/>
-      <c r="F32" s="194"/>
-      <c r="G32" s="194"/>
-      <c r="H32" s="194"/>
-      <c r="I32" s="194"/>
-      <c r="J32" s="194"/>
+      <c r="E32" s="210"/>
+      <c r="F32" s="210"/>
+      <c r="G32" s="210"/>
+      <c r="H32" s="210"/>
+      <c r="I32" s="210"/>
+      <c r="J32" s="210"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="93">
@@ -6148,12 +6149,12 @@
       </c>
       <c r="C33" s="75"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="194"/>
-      <c r="F33" s="194"/>
-      <c r="G33" s="194"/>
-      <c r="H33" s="194"/>
-      <c r="I33" s="194"/>
-      <c r="J33" s="194"/>
+      <c r="E33" s="210"/>
+      <c r="F33" s="210"/>
+      <c r="G33" s="210"/>
+      <c r="H33" s="210"/>
+      <c r="I33" s="210"/>
+      <c r="J33" s="210"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="94">
@@ -6164,12 +6165,12 @@
       </c>
       <c r="C34" s="75"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="194"/>
-      <c r="F34" s="194"/>
-      <c r="G34" s="194"/>
-      <c r="H34" s="194"/>
-      <c r="I34" s="194"/>
-      <c r="J34" s="194"/>
+      <c r="E34" s="210"/>
+      <c r="F34" s="210"/>
+      <c r="G34" s="210"/>
+      <c r="H34" s="210"/>
+      <c r="I34" s="210"/>
+      <c r="J34" s="210"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="95">
@@ -6180,12 +6181,12 @@
       </c>
       <c r="C35" s="75"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="194"/>
-      <c r="F35" s="194"/>
-      <c r="G35" s="194"/>
-      <c r="H35" s="194"/>
-      <c r="I35" s="194"/>
-      <c r="J35" s="194"/>
+      <c r="E35" s="210"/>
+      <c r="F35" s="210"/>
+      <c r="G35" s="210"/>
+      <c r="H35" s="210"/>
+      <c r="I35" s="210"/>
+      <c r="J35" s="210"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="40">
@@ -6196,12 +6197,12 @@
       </c>
       <c r="C36" s="75"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="194"/>
-      <c r="F36" s="194"/>
-      <c r="G36" s="194"/>
-      <c r="H36" s="194"/>
-      <c r="I36" s="194"/>
-      <c r="J36" s="194"/>
+      <c r="E36" s="210"/>
+      <c r="F36" s="210"/>
+      <c r="G36" s="210"/>
+      <c r="H36" s="210"/>
+      <c r="I36" s="210"/>
+      <c r="J36" s="210"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="87">
@@ -6212,12 +6213,12 @@
       </c>
       <c r="C37" s="75"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="194"/>
-      <c r="F37" s="194"/>
-      <c r="G37" s="194"/>
-      <c r="H37" s="194"/>
-      <c r="I37" s="194"/>
-      <c r="J37" s="194"/>
+      <c r="E37" s="210"/>
+      <c r="F37" s="210"/>
+      <c r="G37" s="210"/>
+      <c r="H37" s="210"/>
+      <c r="I37" s="210"/>
+      <c r="J37" s="210"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="88">
@@ -6228,12 +6229,12 @@
       </c>
       <c r="C38" s="75"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="194"/>
-      <c r="F38" s="194"/>
-      <c r="G38" s="194"/>
-      <c r="H38" s="194"/>
-      <c r="I38" s="194"/>
-      <c r="J38" s="194"/>
+      <c r="E38" s="210"/>
+      <c r="F38" s="210"/>
+      <c r="G38" s="210"/>
+      <c r="H38" s="210"/>
+      <c r="I38" s="210"/>
+      <c r="J38" s="210"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="89">
@@ -6244,12 +6245,12 @@
       </c>
       <c r="C39" s="75"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="194"/>
-      <c r="F39" s="194"/>
-      <c r="G39" s="194"/>
-      <c r="H39" s="194"/>
-      <c r="I39" s="194"/>
-      <c r="J39" s="194"/>
+      <c r="E39" s="210"/>
+      <c r="F39" s="210"/>
+      <c r="G39" s="210"/>
+      <c r="H39" s="210"/>
+      <c r="I39" s="210"/>
+      <c r="J39" s="210"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="90">
@@ -6260,12 +6261,12 @@
       </c>
       <c r="C40" s="75"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="194"/>
-      <c r="F40" s="194"/>
-      <c r="G40" s="194"/>
-      <c r="H40" s="194"/>
-      <c r="I40" s="194"/>
-      <c r="J40" s="194"/>
+      <c r="E40" s="210"/>
+      <c r="F40" s="210"/>
+      <c r="G40" s="210"/>
+      <c r="H40" s="210"/>
+      <c r="I40" s="210"/>
+      <c r="J40" s="210"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="91">
@@ -6276,12 +6277,12 @@
       </c>
       <c r="C41" s="75"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="194"/>
-      <c r="F41" s="194"/>
-      <c r="G41" s="194"/>
-      <c r="H41" s="194"/>
-      <c r="I41" s="194"/>
-      <c r="J41" s="194"/>
+      <c r="E41" s="210"/>
+      <c r="F41" s="210"/>
+      <c r="G41" s="210"/>
+      <c r="H41" s="210"/>
+      <c r="I41" s="210"/>
+      <c r="J41" s="210"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="92">
@@ -6292,23 +6293,32 @@
       </c>
       <c r="C42" s="75"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="194"/>
-      <c r="F42" s="194"/>
-      <c r="G42" s="194"/>
-      <c r="H42" s="194"/>
-      <c r="I42" s="194"/>
-      <c r="J42" s="194"/>
+      <c r="E42" s="210"/>
+      <c r="F42" s="210"/>
+      <c r="G42" s="210"/>
+      <c r="H42" s="210"/>
+      <c r="I42" s="210"/>
+      <c r="J42" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -6324,23 +6334,14 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -6382,10 +6383,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -6413,8 +6414,8 @@
       <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -6986,12 +6987,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
       <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
@@ -7021,10 +7022,10 @@
       <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
       <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
@@ -9059,7 +9060,7 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -9083,7 +9084,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="238" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="119"/>
@@ -9117,7 +9118,7 @@
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="234"/>
+      <c r="A2" s="239"/>
       <c r="B2" s="120"/>
       <c r="C2" s="146"/>
       <c r="D2" s="31" t="s">
@@ -9167,15 +9168,15 @@
       <c r="F4" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="204" t="s">
+      <c r="G4" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204" t="s">
+      <c r="H4" s="203"/>
+      <c r="I4" s="203" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
+      <c r="J4" s="203"/>
+      <c r="K4" s="203"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="152">
@@ -9188,21 +9189,21 @@
         <v>51</v>
       </c>
       <c r="D5" s="152"/>
-      <c r="E5" s="153" t="s">
-        <v>230</v>
+      <c r="E5" s="263" t="s">
+        <v>223</v>
       </c>
       <c r="F5" s="154" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="231" t="s">
-        <v>229</v>
-      </c>
-      <c r="H5" s="232"/>
-      <c r="I5" s="235" t="s">
-        <v>228</v>
-      </c>
-      <c r="J5" s="236"/>
-      <c r="K5" s="237"/>
+      <c r="G5" s="236" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" s="237"/>
+      <c r="I5" s="240" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5" s="241"/>
+      <c r="K5" s="242"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="11.25">
       <c r="A6" s="33">
@@ -9213,11 +9214,11 @@
       <c r="D6" s="33"/>
       <c r="E6" s="33"/>
       <c r="F6" s="32"/>
-      <c r="G6" s="238"/>
-      <c r="H6" s="239"/>
-      <c r="I6" s="240"/>
-      <c r="J6" s="241"/>
-      <c r="K6" s="242"/>
+      <c r="G6" s="234"/>
+      <c r="H6" s="235"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="232"/>
+      <c r="K6" s="233"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A7" s="33">
@@ -9228,11 +9229,11 @@
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="238"/>
-      <c r="H7" s="239"/>
-      <c r="I7" s="240"/>
-      <c r="J7" s="241"/>
-      <c r="K7" s="242"/>
+      <c r="G7" s="234"/>
+      <c r="H7" s="235"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="232"/>
+      <c r="K7" s="233"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="33">
@@ -9243,11 +9244,11 @@
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="238"/>
-      <c r="H8" s="239"/>
-      <c r="I8" s="240"/>
-      <c r="J8" s="241"/>
-      <c r="K8" s="242"/>
+      <c r="G8" s="234"/>
+      <c r="H8" s="235"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="232"/>
+      <c r="K8" s="233"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="33">
@@ -9258,11 +9259,11 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="238"/>
-      <c r="H9" s="239"/>
-      <c r="I9" s="240"/>
-      <c r="J9" s="241"/>
-      <c r="K9" s="242"/>
+      <c r="G9" s="234"/>
+      <c r="H9" s="235"/>
+      <c r="I9" s="231"/>
+      <c r="J9" s="232"/>
+      <c r="K9" s="233"/>
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="33">
@@ -9273,11 +9274,11 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="238"/>
-      <c r="H10" s="239"/>
-      <c r="I10" s="240"/>
-      <c r="J10" s="241"/>
-      <c r="K10" s="242"/>
+      <c r="G10" s="234"/>
+      <c r="H10" s="235"/>
+      <c r="I10" s="231"/>
+      <c r="J10" s="232"/>
+      <c r="K10" s="233"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -9288,11 +9289,11 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="238"/>
-      <c r="H11" s="239"/>
-      <c r="I11" s="240"/>
-      <c r="J11" s="241"/>
-      <c r="K11" s="242"/>
+      <c r="G11" s="234"/>
+      <c r="H11" s="235"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="232"/>
+      <c r="K11" s="233"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="33">
@@ -9303,11 +9304,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="238"/>
-      <c r="H12" s="239"/>
-      <c r="I12" s="240"/>
-      <c r="J12" s="241"/>
-      <c r="K12" s="242"/>
+      <c r="G12" s="234"/>
+      <c r="H12" s="235"/>
+      <c r="I12" s="231"/>
+      <c r="J12" s="232"/>
+      <c r="K12" s="233"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -9318,11 +9319,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="238"/>
-      <c r="H13" s="239"/>
-      <c r="I13" s="240"/>
-      <c r="J13" s="241"/>
-      <c r="K13" s="242"/>
+      <c r="G13" s="234"/>
+      <c r="H13" s="235"/>
+      <c r="I13" s="231"/>
+      <c r="J13" s="232"/>
+      <c r="K13" s="233"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -9333,11 +9334,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="238"/>
-      <c r="H14" s="239"/>
-      <c r="I14" s="240"/>
-      <c r="J14" s="241"/>
-      <c r="K14" s="242"/>
+      <c r="G14" s="234"/>
+      <c r="H14" s="235"/>
+      <c r="I14" s="231"/>
+      <c r="J14" s="232"/>
+      <c r="K14" s="233"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -9348,11 +9349,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="238"/>
-      <c r="H15" s="239"/>
-      <c r="I15" s="240"/>
-      <c r="J15" s="241"/>
-      <c r="K15" s="242"/>
+      <c r="G15" s="234"/>
+      <c r="H15" s="235"/>
+      <c r="I15" s="231"/>
+      <c r="J15" s="232"/>
+      <c r="K15" s="233"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="11.25">
       <c r="A16" s="33">
@@ -9363,11 +9364,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="238"/>
-      <c r="H16" s="239"/>
-      <c r="I16" s="240"/>
-      <c r="J16" s="241"/>
-      <c r="K16" s="242"/>
+      <c r="G16" s="234"/>
+      <c r="H16" s="235"/>
+      <c r="I16" s="231"/>
+      <c r="J16" s="232"/>
+      <c r="K16" s="233"/>
     </row>
     <row r="17" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="33">
@@ -9378,11 +9379,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="239"/>
-      <c r="I17" s="240"/>
-      <c r="J17" s="241"/>
-      <c r="K17" s="242"/>
+      <c r="G17" s="234"/>
+      <c r="H17" s="235"/>
+      <c r="I17" s="231"/>
+      <c r="J17" s="232"/>
+      <c r="K17" s="233"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -9393,11 +9394,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="238"/>
-      <c r="H18" s="239"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="241"/>
-      <c r="K18" s="242"/>
+      <c r="G18" s="234"/>
+      <c r="H18" s="235"/>
+      <c r="I18" s="231"/>
+      <c r="J18" s="232"/>
+      <c r="K18" s="233"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -9408,11 +9409,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="238"/>
-      <c r="H19" s="239"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="241"/>
-      <c r="K19" s="242"/>
+      <c r="G19" s="234"/>
+      <c r="H19" s="235"/>
+      <c r="I19" s="231"/>
+      <c r="J19" s="232"/>
+      <c r="K19" s="233"/>
     </row>
     <row r="20" spans="1:19" s="34" customFormat="1" ht="11.25">
       <c r="A20" s="33">
@@ -9423,11 +9424,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="238"/>
-      <c r="H20" s="239"/>
-      <c r="I20" s="240"/>
-      <c r="J20" s="241"/>
-      <c r="K20" s="242"/>
+      <c r="G20" s="234"/>
+      <c r="H20" s="235"/>
+      <c r="I20" s="231"/>
+      <c r="J20" s="232"/>
+      <c r="K20" s="233"/>
     </row>
     <row r="21" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A21" s="33">
@@ -9438,11 +9439,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="195"/>
-      <c r="H21" s="197"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="241"/>
-      <c r="K21" s="242"/>
+      <c r="G21" s="200"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="231"/>
+      <c r="J21" s="232"/>
+      <c r="K21" s="233"/>
     </row>
     <row r="22" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -9453,11 +9454,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="197"/>
-      <c r="I22" s="240"/>
-      <c r="J22" s="241"/>
-      <c r="K22" s="242"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="231"/>
+      <c r="J22" s="232"/>
+      <c r="K22" s="233"/>
     </row>
     <row r="23" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -9468,11 +9469,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="195"/>
-      <c r="H23" s="197"/>
-      <c r="I23" s="240"/>
-      <c r="J23" s="241"/>
-      <c r="K23" s="242"/>
+      <c r="G23" s="200"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="231"/>
+      <c r="J23" s="232"/>
+      <c r="K23" s="233"/>
     </row>
     <row r="24" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -9483,11 +9484,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="195"/>
-      <c r="H24" s="197"/>
-      <c r="I24" s="240"/>
-      <c r="J24" s="241"/>
-      <c r="K24" s="242"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="202"/>
+      <c r="I24" s="231"/>
+      <c r="J24" s="232"/>
+      <c r="K24" s="233"/>
     </row>
     <row r="25" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -9498,11 +9499,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="197"/>
-      <c r="I25" s="240"/>
-      <c r="J25" s="241"/>
-      <c r="K25" s="242"/>
+      <c r="G25" s="200"/>
+      <c r="H25" s="202"/>
+      <c r="I25" s="231"/>
+      <c r="J25" s="232"/>
+      <c r="K25" s="233"/>
     </row>
     <row r="26" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -9513,11 +9514,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="195"/>
-      <c r="H26" s="197"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="241"/>
-      <c r="K26" s="242"/>
+      <c r="G26" s="200"/>
+      <c r="H26" s="202"/>
+      <c r="I26" s="231"/>
+      <c r="J26" s="232"/>
+      <c r="K26" s="233"/>
     </row>
     <row r="27" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -9528,11 +9529,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="195"/>
-      <c r="H27" s="197"/>
-      <c r="I27" s="240"/>
-      <c r="J27" s="241"/>
-      <c r="K27" s="242"/>
+      <c r="G27" s="200"/>
+      <c r="H27" s="202"/>
+      <c r="I27" s="231"/>
+      <c r="J27" s="232"/>
+      <c r="K27" s="233"/>
     </row>
     <row r="28" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -9543,11 +9544,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="195"/>
-      <c r="H28" s="197"/>
-      <c r="I28" s="240"/>
-      <c r="J28" s="241"/>
-      <c r="K28" s="242"/>
+      <c r="G28" s="200"/>
+      <c r="H28" s="202"/>
+      <c r="I28" s="231"/>
+      <c r="J28" s="232"/>
+      <c r="K28" s="233"/>
     </row>
     <row r="29" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A29" s="33">
@@ -9558,11 +9559,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="197"/>
-      <c r="I29" s="240"/>
-      <c r="J29" s="241"/>
-      <c r="K29" s="242"/>
+      <c r="G29" s="200"/>
+      <c r="H29" s="202"/>
+      <c r="I29" s="231"/>
+      <c r="J29" s="232"/>
+      <c r="K29" s="233"/>
     </row>
     <row r="30" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A30" s="33">
@@ -9573,11 +9574,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="195"/>
-      <c r="H30" s="197"/>
-      <c r="I30" s="240"/>
-      <c r="J30" s="241"/>
-      <c r="K30" s="242"/>
+      <c r="G30" s="200"/>
+      <c r="H30" s="202"/>
+      <c r="I30" s="231"/>
+      <c r="J30" s="232"/>
+      <c r="K30" s="233"/>
     </row>
     <row r="31" spans="1:19" ht="11.25">
       <c r="A31" s="33">
@@ -9588,11 +9589,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="197"/>
-      <c r="I31" s="240"/>
-      <c r="J31" s="241"/>
-      <c r="K31" s="242"/>
+      <c r="G31" s="200"/>
+      <c r="H31" s="202"/>
+      <c r="I31" s="231"/>
+      <c r="J31" s="232"/>
+      <c r="K31" s="233"/>
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
       <c r="O31" s="22"/>
@@ -9610,11 +9611,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="197"/>
-      <c r="I32" s="240"/>
-      <c r="J32" s="241"/>
-      <c r="K32" s="242"/>
+      <c r="G32" s="200"/>
+      <c r="H32" s="202"/>
+      <c r="I32" s="231"/>
+      <c r="J32" s="232"/>
+      <c r="K32" s="233"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -9632,11 +9633,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="197"/>
-      <c r="I33" s="240"/>
-      <c r="J33" s="241"/>
-      <c r="K33" s="242"/>
+      <c r="G33" s="200"/>
+      <c r="H33" s="202"/>
+      <c r="I33" s="231"/>
+      <c r="J33" s="232"/>
+      <c r="K33" s="233"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -9654,11 +9655,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="197"/>
-      <c r="I34" s="240"/>
-      <c r="J34" s="241"/>
-      <c r="K34" s="242"/>
+      <c r="G34" s="200"/>
+      <c r="H34" s="202"/>
+      <c r="I34" s="231"/>
+      <c r="J34" s="232"/>
+      <c r="K34" s="233"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -9676,11 +9677,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="197"/>
-      <c r="I35" s="240"/>
-      <c r="J35" s="241"/>
-      <c r="K35" s="242"/>
+      <c r="G35" s="200"/>
+      <c r="H35" s="202"/>
+      <c r="I35" s="231"/>
+      <c r="J35" s="232"/>
+      <c r="K35" s="233"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -9698,11 +9699,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="195"/>
-      <c r="H36" s="197"/>
-      <c r="I36" s="240"/>
-      <c r="J36" s="241"/>
-      <c r="K36" s="242"/>
+      <c r="G36" s="200"/>
+      <c r="H36" s="202"/>
+      <c r="I36" s="231"/>
+      <c r="J36" s="232"/>
+      <c r="K36" s="233"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -9720,11 +9721,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="197"/>
-      <c r="I37" s="240"/>
-      <c r="J37" s="241"/>
-      <c r="K37" s="242"/>
+      <c r="G37" s="200"/>
+      <c r="H37" s="202"/>
+      <c r="I37" s="231"/>
+      <c r="J37" s="232"/>
+      <c r="K37" s="233"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -9742,11 +9743,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="195"/>
-      <c r="H38" s="197"/>
-      <c r="I38" s="240"/>
-      <c r="J38" s="241"/>
-      <c r="K38" s="242"/>
+      <c r="G38" s="200"/>
+      <c r="H38" s="202"/>
+      <c r="I38" s="231"/>
+      <c r="J38" s="232"/>
+      <c r="K38" s="233"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -9764,11 +9765,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="197"/>
-      <c r="I39" s="240"/>
-      <c r="J39" s="241"/>
-      <c r="K39" s="242"/>
+      <c r="G39" s="200"/>
+      <c r="H39" s="202"/>
+      <c r="I39" s="231"/>
+      <c r="J39" s="232"/>
+      <c r="K39" s="233"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -9786,11 +9787,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="197"/>
-      <c r="I40" s="240"/>
-      <c r="J40" s="241"/>
-      <c r="K40" s="242"/>
+      <c r="G40" s="200"/>
+      <c r="H40" s="202"/>
+      <c r="I40" s="231"/>
+      <c r="J40" s="232"/>
+      <c r="K40" s="233"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -9808,11 +9809,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="195"/>
-      <c r="H41" s="197"/>
-      <c r="I41" s="240"/>
-      <c r="J41" s="241"/>
-      <c r="K41" s="242"/>
+      <c r="G41" s="200"/>
+      <c r="H41" s="202"/>
+      <c r="I41" s="231"/>
+      <c r="J41" s="232"/>
+      <c r="K41" s="233"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -9830,11 +9831,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="197"/>
-      <c r="I42" s="240"/>
-      <c r="J42" s="241"/>
-      <c r="K42" s="242"/>
+      <c r="G42" s="200"/>
+      <c r="H42" s="202"/>
+      <c r="I42" s="231"/>
+      <c r="J42" s="232"/>
+      <c r="K42" s="233"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -9852,11 +9853,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="195"/>
-      <c r="H43" s="197"/>
-      <c r="I43" s="240"/>
-      <c r="J43" s="241"/>
-      <c r="K43" s="242"/>
+      <c r="G43" s="200"/>
+      <c r="H43" s="202"/>
+      <c r="I43" s="231"/>
+      <c r="J43" s="232"/>
+      <c r="K43" s="233"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -9874,11 +9875,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="195"/>
-      <c r="H44" s="197"/>
-      <c r="I44" s="240"/>
-      <c r="J44" s="241"/>
-      <c r="K44" s="242"/>
+      <c r="G44" s="200"/>
+      <c r="H44" s="202"/>
+      <c r="I44" s="231"/>
+      <c r="J44" s="232"/>
+      <c r="K44" s="233"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -9896,11 +9897,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="195"/>
-      <c r="H45" s="197"/>
-      <c r="I45" s="240"/>
-      <c r="J45" s="241"/>
-      <c r="K45" s="242"/>
+      <c r="G45" s="200"/>
+      <c r="H45" s="202"/>
+      <c r="I45" s="231"/>
+      <c r="J45" s="232"/>
+      <c r="K45" s="233"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -9918,11 +9919,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="195"/>
-      <c r="H46" s="197"/>
-      <c r="I46" s="240"/>
-      <c r="J46" s="241"/>
-      <c r="K46" s="242"/>
+      <c r="G46" s="200"/>
+      <c r="H46" s="202"/>
+      <c r="I46" s="231"/>
+      <c r="J46" s="232"/>
+      <c r="K46" s="233"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -9940,11 +9941,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="195"/>
-      <c r="H47" s="197"/>
-      <c r="I47" s="240"/>
-      <c r="J47" s="241"/>
-      <c r="K47" s="242"/>
+      <c r="G47" s="200"/>
+      <c r="H47" s="202"/>
+      <c r="I47" s="231"/>
+      <c r="J47" s="232"/>
+      <c r="K47" s="233"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -9962,11 +9963,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="195"/>
-      <c r="H48" s="197"/>
-      <c r="I48" s="240"/>
-      <c r="J48" s="241"/>
-      <c r="K48" s="242"/>
+      <c r="G48" s="200"/>
+      <c r="H48" s="202"/>
+      <c r="I48" s="231"/>
+      <c r="J48" s="232"/>
+      <c r="K48" s="233"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -9984,11 +9985,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="195"/>
-      <c r="H49" s="197"/>
-      <c r="I49" s="240"/>
-      <c r="J49" s="241"/>
-      <c r="K49" s="242"/>
+      <c r="G49" s="200"/>
+      <c r="H49" s="202"/>
+      <c r="I49" s="231"/>
+      <c r="J49" s="232"/>
+      <c r="K49" s="233"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -10006,11 +10007,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="195"/>
-      <c r="H50" s="197"/>
-      <c r="I50" s="240"/>
-      <c r="J50" s="241"/>
-      <c r="K50" s="242"/>
+      <c r="G50" s="200"/>
+      <c r="H50" s="202"/>
+      <c r="I50" s="231"/>
+      <c r="J50" s="232"/>
+      <c r="K50" s="233"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -10028,11 +10029,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="195"/>
-      <c r="H51" s="197"/>
-      <c r="I51" s="240"/>
-      <c r="J51" s="241"/>
-      <c r="K51" s="242"/>
+      <c r="G51" s="200"/>
+      <c r="H51" s="202"/>
+      <c r="I51" s="231"/>
+      <c r="J51" s="232"/>
+      <c r="K51" s="233"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -10050,11 +10051,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="195"/>
-      <c r="H52" s="197"/>
-      <c r="I52" s="240"/>
-      <c r="J52" s="241"/>
-      <c r="K52" s="242"/>
+      <c r="G52" s="200"/>
+      <c r="H52" s="202"/>
+      <c r="I52" s="231"/>
+      <c r="J52" s="232"/>
+      <c r="K52" s="233"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -10072,11 +10073,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="195"/>
-      <c r="H53" s="197"/>
-      <c r="I53" s="240"/>
-      <c r="J53" s="241"/>
-      <c r="K53" s="242"/>
+      <c r="G53" s="200"/>
+      <c r="H53" s="202"/>
+      <c r="I53" s="231"/>
+      <c r="J53" s="232"/>
+      <c r="K53" s="233"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -10094,11 +10095,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="195"/>
-      <c r="H54" s="197"/>
-      <c r="I54" s="240"/>
-      <c r="J54" s="241"/>
-      <c r="K54" s="242"/>
+      <c r="G54" s="200"/>
+      <c r="H54" s="202"/>
+      <c r="I54" s="231"/>
+      <c r="J54" s="232"/>
+      <c r="K54" s="233"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -10116,11 +10117,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="195"/>
-      <c r="H55" s="197"/>
-      <c r="I55" s="240"/>
-      <c r="J55" s="241"/>
-      <c r="K55" s="242"/>
+      <c r="G55" s="200"/>
+      <c r="H55" s="202"/>
+      <c r="I55" s="231"/>
+      <c r="J55" s="232"/>
+      <c r="K55" s="233"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -10132,6 +10133,97 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="105">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="G52:H52"/>
     <mergeCell ref="G53:H53"/>
@@ -10146,97 +10238,6 @@
     <mergeCell ref="I53:K53"/>
     <mergeCell ref="I54:K54"/>
     <mergeCell ref="I55:K55"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F55">
@@ -10254,8 +10255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1048467"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="H7" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="H7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -10283,24 +10284,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="249" t="str">
+      <c r="J1" s="246" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="K1" s="249"/>
+      <c r="K1" s="246"/>
       <c r="L1" s="26" t="s">
         <v>3</v>
       </c>
@@ -10325,22 +10326,22 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="249" t="str">
+      <c r="J2" s="246" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - T</v>
       </c>
-      <c r="K2" s="249"/>
+      <c r="K2" s="246"/>
       <c r="L2" s="26" t="s">
         <v>49</v>
       </c>
@@ -10395,12 +10396,12 @@
       <c r="J4" s="147" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="250" t="s">
+      <c r="K4" s="247" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="251"/>
-      <c r="M4" s="251"/>
-      <c r="N4" s="252"/>
+      <c r="L4" s="248"/>
+      <c r="M4" s="248"/>
+      <c r="N4" s="249"/>
       <c r="O4" s="147" t="s">
         <v>56</v>
       </c>
@@ -10440,12 +10441,12 @@
       <c r="J5" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="K5" s="201" t="s">
+      <c r="K5" s="197" t="s">
         <v>179</v>
       </c>
-      <c r="L5" s="202"/>
-      <c r="M5" s="202"/>
-      <c r="N5" s="203"/>
+      <c r="L5" s="198"/>
+      <c r="M5" s="198"/>
+      <c r="N5" s="199"/>
       <c r="O5" s="121" t="s">
         <v>181</v>
       </c>
@@ -10487,12 +10488,12 @@
       <c r="J6" s="134" t="s">
         <v>191</v>
       </c>
-      <c r="K6" s="246" t="s">
+      <c r="K6" s="250" t="s">
         <v>194</v>
       </c>
-      <c r="L6" s="247"/>
-      <c r="M6" s="247"/>
-      <c r="N6" s="248"/>
+      <c r="L6" s="251"/>
+      <c r="M6" s="251"/>
+      <c r="N6" s="252"/>
       <c r="O6" s="135" t="s">
         <v>193</v>
       </c>
@@ -10533,12 +10534,12 @@
       <c r="J7" s="134" t="s">
         <v>196</v>
       </c>
-      <c r="K7" s="246" t="s">
+      <c r="K7" s="250" t="s">
         <v>188</v>
       </c>
-      <c r="L7" s="247"/>
-      <c r="M7" s="247"/>
-      <c r="N7" s="248"/>
+      <c r="L7" s="251"/>
+      <c r="M7" s="251"/>
+      <c r="N7" s="252"/>
       <c r="O7" s="135" t="s">
         <v>189</v>
       </c>
@@ -10564,13 +10565,13 @@
         <v>51</v>
       </c>
       <c r="D8" s="161" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E8" s="161" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F8" s="156" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G8" s="155" t="s">
         <v>212</v>
@@ -10585,25 +10586,25 @@
         <v>213</v>
       </c>
       <c r="K8" s="253" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="L8" s="254"/>
       <c r="M8" s="254"/>
       <c r="N8" s="255"/>
       <c r="O8" s="158" t="s">
+        <v>226</v>
+      </c>
+      <c r="P8" s="158" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q8" s="156" t="s">
         <v>214</v>
       </c>
-      <c r="P8" s="158" t="s">
+      <c r="R8" s="155" t="s">
         <v>215</v>
       </c>
-      <c r="Q8" s="156" t="s">
-        <v>216</v>
-      </c>
-      <c r="R8" s="155" t="s">
-        <v>217</v>
-      </c>
       <c r="S8" s="159" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="T8" s="162"/>
       <c r="U8" s="162"/>
@@ -10646,10 +10647,10 @@
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
-      <c r="K10" s="240"/>
-      <c r="L10" s="241"/>
-      <c r="M10" s="241"/>
-      <c r="N10" s="242"/>
+      <c r="K10" s="231"/>
+      <c r="L10" s="232"/>
+      <c r="M10" s="232"/>
+      <c r="N10" s="233"/>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
@@ -12702,36 +12703,54 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="94">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="K87:N87"/>
+    <mergeCell ref="K61:N61"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="K63:N63"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="K66:N66"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K93:N93"/>
+    <mergeCell ref="K77:N77"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K89:N89"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="K94:N94"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="K79:N79"/>
+    <mergeCell ref="K80:N80"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="K82:N82"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K85:N85"/>
+    <mergeCell ref="K86:N86"/>
+    <mergeCell ref="K69:N69"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="K71:N71"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="K53:N53"/>
     <mergeCell ref="K58:N58"/>
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="K34:N34"/>
@@ -12748,54 +12767,36 @@
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="K48:N48"/>
     <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K94:N94"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K79:N79"/>
-    <mergeCell ref="K80:N80"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K82:N82"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K85:N85"/>
-    <mergeCell ref="K86:N86"/>
-    <mergeCell ref="K69:N69"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="K93:N93"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K89:N89"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="K87:N87"/>
-    <mergeCell ref="K61:N61"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="K63:N63"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048467:Q1048576 Q5:Q9 Q11:Q94"/>
@@ -12824,8 +12825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -12841,10 +12842,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12872,8 +12873,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13021,13 +13022,13 @@
     </row>
     <row r="13" spans="1:10" s="151" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="151" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B13" s="151" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D13" s="160" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
@@ -13270,7 +13271,7 @@
       </c>
       <c r="B32" s="165"/>
       <c r="C32" s="165" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D32" s="165"/>
       <c r="E32" s="165"/>
@@ -13283,7 +13284,7 @@
     <row r="33" spans="1:10" s="125" customFormat="1" ht="12" customHeight="1">
       <c r="A33" s="164"/>
       <c r="B33" s="167" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C33" s="165"/>
       <c r="D33" s="165"/>
@@ -13308,9 +13309,7 @@
     </row>
     <row r="35" spans="1:10" s="125" customFormat="1" ht="12" customHeight="1">
       <c r="A35" s="164"/>
-      <c r="B35" s="167" t="s">
-        <v>224</v>
-      </c>
+      <c r="B35" s="167"/>
       <c r="C35" s="165"/>
       <c r="D35" s="165"/>
       <c r="E35" s="165"/>
@@ -14085,10 +14084,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="204"/>
+      <c r="B1" s="203"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -14116,8 +14115,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>